<commit_message>
30.06.2020 MC Last Update
</commit_message>
<xml_diff>
--- a/2020/June/All Details/30.06.2020/MC Bank Statement June 2020.xlsx
+++ b/2020/June/All Details/30.06.2020/MC Bank Statement June 2020.xlsx
@@ -1603,7 +1603,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1615,7 +1615,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1638,14 +1638,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3185,8 +3185,8 @@
   </sheetPr>
   <dimension ref="A1:AL222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" customHeight="1"/>
@@ -3315,7 +3315,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="108">
-        <v>190794.86749999999</v>
+        <v>208927.94750000001</v>
       </c>
       <c r="F4" s="89"/>
       <c r="G4" s="66"/>
@@ -3356,7 +3356,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="107">
-        <v>295155.30500000011</v>
+        <v>297489.90500000009</v>
       </c>
       <c r="C5" s="107"/>
       <c r="D5" s="101" t="s">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B6" s="107">
         <f>B4+B5</f>
-        <v>6795523.3049999997</v>
+        <v>6797857.9050000003</v>
       </c>
       <c r="C6" s="101"/>
       <c r="D6" s="101" t="s">
@@ -3554,7 +3554,7 @@
         <v>62</v>
       </c>
       <c r="E9" s="108">
-        <v>351624.4375</v>
+        <v>335825.95750000048</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="66" t="s">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="B10" s="112">
         <f>B5-B8-B9</f>
-        <v>204770.30500000011</v>
+        <v>207104.90500000009</v>
       </c>
       <c r="C10" s="103"/>
       <c r="D10" s="101"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="B13" s="113">
         <f>B6-B8-B11+B12-B9</f>
-        <v>6605138.3049999997</v>
+        <v>6607472.9050000003</v>
       </c>
       <c r="C13" s="105"/>
       <c r="D13" s="105" t="s">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="E13" s="114">
         <f>E4+E5+E6+E7+E8-E11+E9-E10</f>
-        <v>6605138.3049999997</v>
+        <v>6607472.9050000003</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="63">

</xml_diff>